<commit_message>
datos de productos, clientes, proveedores
</commit_message>
<xml_diff>
--- a/docs/data_informacion.xlsx
+++ b/docs/data_informacion.xlsx
@@ -5,15 +5,19 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Proyecto__Tesis\ProdeFarm\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\ProdeFarm\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AA15891-A2B4-41A0-B617-C1F579CCF74A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB821A14-FDB7-4201-B38E-30D1A1B3A532}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11760" xr2:uid="{C7B42AE2-71C8-4403-B8BF-033F16041F11}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{C7B42AE2-71C8-4403-B8BF-033F16041F11}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Categoria" sheetId="1" r:id="rId1"/>
+    <sheet name="Producto" sheetId="3" r:id="rId2"/>
+    <sheet name="Proveedores" sheetId="4" r:id="rId3"/>
+    <sheet name="unidades medida" sheetId="5" r:id="rId4"/>
+    <sheet name="Clientes" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="72">
   <si>
     <t>CAT_ID</t>
   </si>
@@ -60,6 +64,198 @@
   </si>
   <si>
     <t>Bienestar Sexual</t>
+  </si>
+  <si>
+    <t>CLI_ID</t>
+  </si>
+  <si>
+    <t>EMP_ID</t>
+  </si>
+  <si>
+    <t>CLI_NOM</t>
+  </si>
+  <si>
+    <t>CLI_RUC</t>
+  </si>
+  <si>
+    <t>CLI_TELF</t>
+  </si>
+  <si>
+    <t>CLI_DIRECC</t>
+  </si>
+  <si>
+    <t>CLI_CORREO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABARCA STRONG ELENA  </t>
+  </si>
+  <si>
+    <t>Guayaquil</t>
+  </si>
+  <si>
+    <t xml:space="preserve">polaab@hotmail.com  </t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIL ELSA  </t>
+  </si>
+  <si>
+    <t>Kennedy norte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">elsaabril5140@gmail.com  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABRIL ORTIZ KATHY  </t>
+  </si>
+  <si>
+    <t>bastion popular</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emmaabril@yahoo.com  </t>
+  </si>
+  <si>
+    <t>NACELDO ENRIQUEZ GEOCONDA PAULINA  ULL</t>
+  </si>
+  <si>
+    <t>alborada</t>
+  </si>
+  <si>
+    <t xml:space="preserve">chiquipauli.22@hotmail.com  </t>
+  </si>
+  <si>
+    <t>PROD_ID</t>
+  </si>
+  <si>
+    <t>PROD_NOM</t>
+  </si>
+  <si>
+    <t>PROD_DESCRIP</t>
+  </si>
+  <si>
+    <t>UND_ID</t>
+  </si>
+  <si>
+    <t>PROD_PCOMPRA</t>
+  </si>
+  <si>
+    <t>PROD_PVENTA</t>
+  </si>
+  <si>
+    <t>PROD_STOCK</t>
+  </si>
+  <si>
+    <t>PROD_FECHVEN</t>
+  </si>
+  <si>
+    <t>PROD_IMG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUPETES  VITAMINA C CAJAX10  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUPETES DE VITAMINA C +ZINC  CAJAX10  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHUPETES DE VITAMINA C +ZINC CAJAX10  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARAMELOS VITAMINA C+ZINC+VITAMINA D CAJA X 30  90G  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEC-M SPRAY 90 ML  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PARA EL CUIDADO DE LOS HONGOS  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">WEC-M TALCO 45GR  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CONTROLA EL SUDOR Y EL MAL OLOR  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SABELL JABON DE MATICO 75GR  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">EXTRACTO DE MATICO DESINFLAMATORIO  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUDENCE MIX CAJAX3  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUDENCE EFECTO RETARDANTE CAJAX3  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PRUDENCE ULTRA SENSIBLE CAJAX3  </t>
+  </si>
+  <si>
+    <t>PROV_ID</t>
+  </si>
+  <si>
+    <t>PROV_NOM</t>
+  </si>
+  <si>
+    <t>PROV_RUC</t>
+  </si>
+  <si>
+    <t>PROV_TELF</t>
+  </si>
+  <si>
+    <t>PROV_DIRECC</t>
+  </si>
+  <si>
+    <t>PROV_CORREO</t>
+  </si>
+  <si>
+    <t>ALL MEDIC ECUADOR SCRUBS</t>
+  </si>
+  <si>
+    <t>Quito</t>
+  </si>
+  <si>
+    <t>Scrubs@medic.com</t>
+  </si>
+  <si>
+    <t>ALMERCATO S.A.S.</t>
+  </si>
+  <si>
+    <t>Samanes</t>
+  </si>
+  <si>
+    <t>Almercato@marketing@.com</t>
+  </si>
+  <si>
+    <t>ALTAMIRANO ROJAS MARIA BERTHA</t>
+  </si>
+  <si>
+    <t>Los Rios</t>
+  </si>
+  <si>
+    <t>atalmrs@cobranzas.com</t>
+  </si>
+  <si>
+    <t>ALNUSAL CIA LTDA</t>
+  </si>
+  <si>
+    <t>Cuenca</t>
+  </si>
+  <si>
+    <t>contabilidad@nunezsanchez.com.ec</t>
+  </si>
+  <si>
+    <t>UND_NOM</t>
+  </si>
+  <si>
+    <t>Unidad</t>
+  </si>
+  <si>
+    <t>Caja</t>
+  </si>
+  <si>
+    <t>Docena</t>
   </si>
 </sst>
 </file>
@@ -413,16 +609,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37EECC8F-07DA-48F3-BE13-09BFFF852F18}">
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="18.5546875" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -439,7 +635,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B2">
         <v>1</v>
       </c>
@@ -450,7 +646,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B3">
         <v>1</v>
       </c>
@@ -461,7 +657,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4">
         <v>1</v>
       </c>
@@ -472,7 +668,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5">
         <v>2</v>
       </c>
@@ -483,7 +679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>2</v>
       </c>
@@ -494,7 +690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -505,7 +701,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>3</v>
       </c>
@@ -516,7 +712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>3</v>
       </c>
@@ -527,7 +723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>3</v>
       </c>
@@ -538,7 +734,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>4</v>
       </c>
@@ -549,7 +745,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>4</v>
       </c>
@@ -560,7 +756,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>4</v>
       </c>
@@ -569,6 +765,1229 @@
       </c>
       <c r="E13">
         <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1A6DE3-3995-4B39-B402-11FDE4D06699}">
+  <dimension ref="A1:M10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="44.85546875" customWidth="1"/>
+    <col min="5" max="5" width="39.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G1" t="s">
+        <v>32</v>
+      </c>
+      <c r="H1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>36</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>0.75</v>
+      </c>
+      <c r="H2">
+        <v>1.45</v>
+      </c>
+      <c r="I2">
+        <v>50</v>
+      </c>
+      <c r="J2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" t="s">
+        <v>18</v>
+      </c>
+      <c r="L2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3">
+        <v>2</v>
+      </c>
+      <c r="G3">
+        <v>0.65</v>
+      </c>
+      <c r="H3">
+        <v>1.3</v>
+      </c>
+      <c r="I3">
+        <v>50</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>18</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4">
+        <v>0.8</v>
+      </c>
+      <c r="H4">
+        <v>1.7</v>
+      </c>
+      <c r="I4">
+        <v>50</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" t="s">
+        <v>42</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5">
+        <v>2.35</v>
+      </c>
+      <c r="H5">
+        <v>3.7</v>
+      </c>
+      <c r="I5">
+        <v>50</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>18</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>44</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6">
+        <v>1.55</v>
+      </c>
+      <c r="H6">
+        <v>2.5</v>
+      </c>
+      <c r="I6">
+        <v>50</v>
+      </c>
+      <c r="J6" t="s">
+        <v>18</v>
+      </c>
+      <c r="K6" t="s">
+        <v>18</v>
+      </c>
+      <c r="L6" t="s">
+        <v>18</v>
+      </c>
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E7" t="s">
+        <v>46</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H7">
+        <v>1.5</v>
+      </c>
+      <c r="I7">
+        <v>50</v>
+      </c>
+      <c r="J7" t="s">
+        <v>18</v>
+      </c>
+      <c r="K7" t="s">
+        <v>18</v>
+      </c>
+      <c r="L7" t="s">
+        <v>18</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>3</v>
+      </c>
+      <c r="D8" t="s">
+        <v>47</v>
+      </c>
+      <c r="E8" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8">
+        <v>2</v>
+      </c>
+      <c r="G8">
+        <v>3.2</v>
+      </c>
+      <c r="H8">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I8">
+        <v>50</v>
+      </c>
+      <c r="J8" t="s">
+        <v>18</v>
+      </c>
+      <c r="K8" t="s">
+        <v>18</v>
+      </c>
+      <c r="L8" t="s">
+        <v>18</v>
+      </c>
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>3</v>
+      </c>
+      <c r="D9" t="s">
+        <v>48</v>
+      </c>
+      <c r="E9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F9">
+        <v>2</v>
+      </c>
+      <c r="G9">
+        <v>3.2</v>
+      </c>
+      <c r="H9">
+        <v>4.5999999999999996</v>
+      </c>
+      <c r="I9">
+        <v>50</v>
+      </c>
+      <c r="J9" t="s">
+        <v>18</v>
+      </c>
+      <c r="K9" t="s">
+        <v>18</v>
+      </c>
+      <c r="L9" t="s">
+        <v>18</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
+        <v>49</v>
+      </c>
+      <c r="F10">
+        <v>2</v>
+      </c>
+      <c r="G10">
+        <v>3.6</v>
+      </c>
+      <c r="H10">
+        <v>5.0999999999999996</v>
+      </c>
+      <c r="I10">
+        <v>50</v>
+      </c>
+      <c r="J10" t="s">
+        <v>18</v>
+      </c>
+      <c r="K10" t="s">
+        <v>18</v>
+      </c>
+      <c r="L10" t="s">
+        <v>18</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3159824-39E3-4CA2-A044-A2B1F90D589D}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="37.85546875" customWidth="1"/>
+    <col min="4" max="4" width="29.7109375" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" customWidth="1"/>
+    <col min="7" max="7" width="34.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2">
+        <v>956894525001</v>
+      </c>
+      <c r="E2">
+        <v>956745392</v>
+      </c>
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3">
+        <v>1793648724001</v>
+      </c>
+      <c r="E3">
+        <v>946746392</v>
+      </c>
+      <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4">
+        <v>108346215</v>
+      </c>
+      <c r="E4">
+        <v>2840340</v>
+      </c>
+      <c r="F4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G4" t="s">
+        <v>64</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>65</v>
+      </c>
+      <c r="D5">
+        <v>1700982322301</v>
+      </c>
+      <c r="E5">
+        <v>978653422</v>
+      </c>
+      <c r="F5" t="s">
+        <v>66</v>
+      </c>
+      <c r="G5" t="s">
+        <v>67</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6">
+        <v>956894525001</v>
+      </c>
+      <c r="E6">
+        <v>956745392</v>
+      </c>
+      <c r="F6" t="s">
+        <v>57</v>
+      </c>
+      <c r="G6" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>59</v>
+      </c>
+      <c r="D7">
+        <v>1793648724001</v>
+      </c>
+      <c r="E7">
+        <v>946746392</v>
+      </c>
+      <c r="F7" t="s">
+        <v>60</v>
+      </c>
+      <c r="G7" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8">
+        <v>108346215</v>
+      </c>
+      <c r="E8">
+        <v>2840340</v>
+      </c>
+      <c r="F8" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9">
+        <v>1700982322301</v>
+      </c>
+      <c r="E9">
+        <v>978653422</v>
+      </c>
+      <c r="F9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G9" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1197AD26-F561-4AD4-82F8-EE74077F8AE8}">
+  <dimension ref="A1:E13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>70</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>70</v>
+      </c>
+      <c r="D6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>69</v>
+      </c>
+      <c r="D8" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="C10" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>6</v>
+      </c>
+      <c r="C11" t="s">
+        <v>69</v>
+      </c>
+      <c r="D11" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>6</v>
+      </c>
+      <c r="C12" t="s">
+        <v>70</v>
+      </c>
+      <c r="D12" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="C13" t="s">
+        <v>71</v>
+      </c>
+      <c r="D13" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8399FF4A-1D9D-46AE-A871-C8C1EAA4DD2C}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2">
+        <v>903407302</v>
+      </c>
+      <c r="E2">
+        <v>3082070</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3">
+        <v>2100116314</v>
+      </c>
+      <c r="E3">
+        <v>2820469</v>
+      </c>
+      <c r="F3" t="s">
+        <v>20</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>1713721114</v>
+      </c>
+      <c r="E4">
+        <v>44610826</v>
+      </c>
+      <c r="F4" t="s">
+        <v>23</v>
+      </c>
+      <c r="G4" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5">
+        <v>1720888617001</v>
+      </c>
+      <c r="E5">
+        <v>3020734</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2</v>
+      </c>
+      <c r="C6" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6">
+        <v>903407302</v>
+      </c>
+      <c r="E6">
+        <v>3082070</v>
+      </c>
+      <c r="F6" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>2</v>
+      </c>
+      <c r="C7" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7">
+        <v>2100116314</v>
+      </c>
+      <c r="E7">
+        <v>2820469</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>2</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8">
+        <v>1713721114</v>
+      </c>
+      <c r="E8">
+        <v>44610826</v>
+      </c>
+      <c r="F8" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H8" t="s">
+        <v>18</v>
+      </c>
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>25</v>
+      </c>
+      <c r="D9">
+        <v>1720888617001</v>
+      </c>
+      <c r="E9">
+        <v>3020734</v>
+      </c>
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G9" t="s">
+        <v>27</v>
+      </c>
+      <c r="H9" t="s">
+        <v>18</v>
+      </c>
+      <c r="I9" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>